<commit_message>
Changes to be committed: 	modified:   ANALISIS SISTEM/database.xlsx 	modified:   backend/simprosis/olahDataMahasiswa/forms.py 	modified:   backend/simprosis/olahDataMahasiswa/models.py 	modified:   backend/simprosis/olahDataMahasiswa/views.py 	modified:   backend/simprosis/rps/forms.py 	modified:   backend/simprosis/rps/urls.py 	modified:   backend/simprosis/rps/views.py
Untracked files:
	ANALISIS SISTEM/~$database.xlsx
	backend/simprosis/rps/templates/rps/fakultas_form.html
	backend/simprosis/rps/templates/rps/fakultas_list.html
	backend/simprosis/static/vendor/jquery/jquery.formset.js
</commit_message>
<xml_diff>
--- a/ANALISIS SISTEM/database.xlsx
+++ b/ANALISIS SISTEM/database.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KERJA\UNP\PRODI\prjsiunp\ANALISIS SISTEM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14840" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14835" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="95">
   <si>
     <t>mahasiswa</t>
   </si>
@@ -219,21 +224,6 @@
     <t>indikator</t>
   </si>
   <si>
-    <t xml:space="preserve">materi </t>
-  </si>
-  <si>
-    <t>bentukBelajar</t>
-  </si>
-  <si>
-    <t>jenisPenilaian</t>
-  </si>
-  <si>
-    <t>kriteriaPenilaian</t>
-  </si>
-  <si>
-    <t>bobot</t>
-  </si>
-  <si>
     <t>referensi</t>
   </si>
   <si>
@@ -265,13 +255,67 @@
   </si>
   <si>
     <t>jmlPertemuan</t>
+  </si>
+  <si>
+    <t>+ rumpun</t>
+  </si>
+  <si>
+    <t>tanggalPenyusunan</t>
+  </si>
+  <si>
+    <t>kaprodi</t>
+  </si>
+  <si>
+    <t>cpProdi</t>
+  </si>
+  <si>
+    <t>cpMk</t>
+  </si>
+  <si>
+    <t>materiPembelajaran</t>
+  </si>
+  <si>
+    <t>idRef</t>
+  </si>
+  <si>
+    <t>mediaBelajar</t>
+  </si>
+  <si>
+    <t>teamTeaching</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>materiBelajar</t>
+  </si>
+  <si>
+    <t>bentukMetode</t>
+  </si>
+  <si>
+    <t>pengalamanBelajarOffline</t>
+  </si>
+  <si>
+    <t>pengalamanBelajarOnlineSinkron</t>
+  </si>
+  <si>
+    <t>pengalamanBelajarOnlineAsinkron</t>
+  </si>
+  <si>
+    <t>teknikPenilaian</t>
+  </si>
+  <si>
+    <t>indikatorPenilaian</t>
+  </si>
+  <si>
+    <t>bobotPenilaian</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -291,6 +335,13 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -397,9 +448,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -409,11 +466,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -440,6 +494,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -767,41 +829,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="1" max="1" width="3.375" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="4" max="4" width="4.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1"/>
-    <col min="7" max="7" width="5.33203125" customWidth="1"/>
-    <col min="10" max="10" width="4.33203125" customWidth="1"/>
-    <col min="13" max="13" width="6.6640625" customWidth="1"/>
+    <col min="4" max="4" width="4.625" customWidth="1"/>
+    <col min="5" max="5" width="12.375" customWidth="1"/>
+    <col min="7" max="7" width="5.375" customWidth="1"/>
+    <col min="10" max="10" width="4.375" customWidth="1"/>
+    <col min="13" max="13" width="6.625" customWidth="1"/>
+    <col min="14" max="14" width="13.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15">
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="E2" s="4" t="s">
+      <c r="C2" s="7"/>
+      <c r="E2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="H2" s="4" t="s">
+      <c r="F2" s="8"/>
+      <c r="H2" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="K2" s="4" t="s">
+      <c r="I2" s="8"/>
+      <c r="K2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="5"/>
-    </row>
-    <row r="3" spans="2:15">
+      <c r="L2" s="8"/>
+      <c r="M2" s="2"/>
+      <c r="N2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -826,9 +892,15 @@
       <c r="L3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="6"/>
-    </row>
-    <row r="4" spans="2:15">
+      <c r="M3" s="3"/>
+      <c r="N3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -853,9 +925,15 @@
       <c r="L4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M4" s="6"/>
-    </row>
-    <row r="5" spans="2:15">
+      <c r="M4" s="3"/>
+      <c r="N4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -880,9 +958,15 @@
       <c r="L5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M5" s="6"/>
-    </row>
-    <row r="6" spans="2:15">
+      <c r="M5" s="3"/>
+      <c r="N5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -907,13 +991,19 @@
       <c r="L6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M6" s="6"/>
-    </row>
-    <row r="7" spans="2:15">
-      <c r="B7" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="C7" s="7" t="s">
+      <c r="M6" s="3"/>
+      <c r="N6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -928,32 +1018,56 @@
       <c r="L7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M7" s="6"/>
-    </row>
-    <row r="8" spans="2:15">
+      <c r="M7" s="3"/>
+      <c r="N7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="K8" s="1" t="s">
         <v>43</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M8" s="6"/>
-    </row>
-    <row r="9" spans="2:15">
-      <c r="E9" s="4" t="s">
+      <c r="M8" s="3"/>
+      <c r="N8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="E9" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="H9" s="4" t="s">
+      <c r="F9" s="8"/>
+      <c r="H9" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="2:15">
-      <c r="B10" s="2" t="s">
+      <c r="I9" s="8"/>
+      <c r="N9" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="7"/>
       <c r="E10" s="1" t="s">
         <v>19</v>
       </c>
@@ -966,15 +1080,15 @@
       <c r="I10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="K10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="L10" s="4"/>
-      <c r="N10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15">
+      <c r="L10" s="8"/>
+      <c r="N10" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
@@ -999,14 +1113,14 @@
       <c r="L11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N11" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:15">
+      <c r="N11" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="O11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
@@ -1025,14 +1139,14 @@
       <c r="L12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N12" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15">
+      <c r="N12" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="O12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
@@ -1051,32 +1165,29 @@
       <c r="L13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="N13" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15">
+      <c r="N13" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="O13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="K14" s="1" t="s">
         <v>22</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N14" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="O14" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:15">
-      <c r="E15" s="4" t="s">
+      <c r="N14" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="E15" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F15" s="4"/>
+      <c r="F15" s="8"/>
       <c r="H15" t="s">
         <v>57</v>
       </c>
@@ -1086,18 +1197,18 @@
       <c r="L15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N15" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="2:15">
-      <c r="B16" s="2" t="s">
+      <c r="N15" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="O15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="3"/>
+      <c r="C16" s="7"/>
       <c r="E16" s="1" t="s">
         <v>34</v>
       </c>
@@ -1116,14 +1227,14 @@
       <c r="L16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N16" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="2:15">
+      <c r="N16" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="O16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1149,7 +1260,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="2:15">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1168,15 +1279,15 @@
       <c r="I18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7" t="s">
+      <c r="K18" s="4"/>
+      <c r="L18" s="4" t="s">
         <v>7</v>
       </c>
       <c r="N18" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="2:15">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E19" s="1" t="s">
         <v>36</v>
       </c>
@@ -1190,17 +1301,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="2:15">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E20" s="1" t="s">
         <v>37</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K20" s="4" t="s">
+      <c r="K20" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="L20" s="4"/>
+      <c r="L20" s="8"/>
       <c r="N20" s="1" t="s">
         <v>64</v>
       </c>
@@ -1208,7 +1319,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="2:15">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E21" s="1" t="s">
         <v>39</v>
       </c>
@@ -1228,7 +1339,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="2:15">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E22" s="1" t="s">
         <v>40</v>
       </c>
@@ -1242,13 +1353,13 @@
         <v>44</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="O22" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="2:15">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E23" s="1" t="s">
         <v>41</v>
       </c>
@@ -1262,108 +1373,106 @@
         <v>6</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="O23" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="2:15">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E24" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="N24" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="O24" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="2:15">
+      <c r="N24" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="O24" s="10"/>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H25" t="s">
-        <v>71</v>
-      </c>
-      <c r="N25" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="O25" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="2:15">
+        <v>66</v>
+      </c>
+      <c r="N25" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="O25" s="10"/>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H26" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N26" s="1" t="s">
+      <c r="N26" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="O26" s="10"/>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H27" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="N27" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="O27" s="10"/>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H28" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N28" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H29" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N29" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H30" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="O26" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="2:15">
-      <c r="H27" s="1" t="s">
+      <c r="I30" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H31" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H32" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H33" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="N27" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="O27" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" spans="2:15">
-      <c r="H28" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="2:15">
-      <c r="H29" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="2:15">
-      <c r="H30" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="2:15">
-      <c r="H31" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="2:15">
-      <c r="H32" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="8:9">
-      <c r="H33" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>6</v>
@@ -1384,7 +1493,7 @@
     <mergeCell ref="E9:F9"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
perubahan model rps Changes to be committed: 	modified:   ANALISIS SISTEM/database.xlsx 	new file:   backend/simprosis/olahDataMahasiswa/migrations/0003_auto_20200305_1047.py 	modified:   backend/simprosis/olahDataMahasiswa/models.py 	modified:   backend/simprosis/olahDataMatakuliah/forms.py 	new file:   backend/simprosis/olahDataMatakuliah/migrations/0010_matakuliah_rumpunmatakuliah.py 	modified:   backend/simprosis/olahDataMatakuliah/models.py 	modified:   backend/simprosis/olahDataMatakuliah/views.py 	modified:   backend/simprosis/olahDataRPS/forms.py 	new file:   backend/simprosis/olahDataRPS/migrations/0014_auto_20200305_1047.py 	new file:   backend/simprosis/olahDataRPS/migrations/0015_auto_20200305_1332.py 	new file:   backend/simprosis/olahDataRPS/migrations/0016_auto_20200305_1358.py 	modified:   backend/simprosis/olahDataRPS/models.py 	modified:   backend/simprosis/olahDataRPS/views.py 	new file:   backend/simprosis/rps/templates/rps/fakultas_confirm_delete.html
</commit_message>
<xml_diff>
--- a/ANALISIS SISTEM/database.xlsx
+++ b/ANALISIS SISTEM/database.xlsx
@@ -290,9 +290,6 @@
     <t>materiBelajar</t>
   </si>
   <si>
-    <t>bentukMetode</t>
-  </si>
-  <si>
     <t>pengalamanBelajarOffline</t>
   </si>
   <si>
@@ -309,6 +306,9 @@
   </si>
   <si>
     <t>bobotPenilaian</t>
+  </si>
+  <si>
+    <t>bentukMetodeBelajar</t>
   </si>
 </sst>
 </file>
@@ -457,17 +457,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -829,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -846,10 +846,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7"/>
+      <c r="C2" s="10"/>
       <c r="E2" s="8" t="s">
         <v>0</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>62</v>
       </c>
       <c r="I9" s="8"/>
-      <c r="N9" s="9" t="s">
+      <c r="N9" s="6" t="s">
         <v>78</v>
       </c>
       <c r="O9" s="4" t="s">
@@ -1064,10 +1064,10 @@
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="7"/>
+      <c r="C10" s="10"/>
       <c r="E10" s="1" t="s">
         <v>19</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>26</v>
       </c>
       <c r="L10" s="8"/>
-      <c r="N10" s="9" t="s">
+      <c r="N10" s="6" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1113,7 +1113,7 @@
       <c r="L11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N11" s="9" t="s">
+      <c r="N11" s="6" t="s">
         <v>80</v>
       </c>
       <c r="O11" t="s">
@@ -1139,7 +1139,7 @@
       <c r="L12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N12" s="9" t="s">
+      <c r="N12" s="6" t="s">
         <v>81</v>
       </c>
       <c r="O12" t="s">
@@ -1165,7 +1165,7 @@
       <c r="L13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="N13" s="9" t="s">
+      <c r="N13" s="6" t="s">
         <v>82</v>
       </c>
       <c r="O13" t="s">
@@ -1179,7 +1179,7 @@
       <c r="L14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N14" s="9" t="s">
+      <c r="N14" s="6" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1197,7 +1197,7 @@
       <c r="L15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N15" s="9" t="s">
+      <c r="N15" s="6" t="s">
         <v>84</v>
       </c>
       <c r="O15" t="s">
@@ -1205,10 +1205,10 @@
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="7"/>
+      <c r="C16" s="10"/>
       <c r="E16" s="1" t="s">
         <v>34</v>
       </c>
@@ -1227,7 +1227,7 @@
       <c r="L16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N16" s="9" t="s">
+      <c r="N16" s="6" t="s">
         <v>85</v>
       </c>
       <c r="O16" t="s">
@@ -1373,7 +1373,7 @@
         <v>6</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="O23" s="1" t="s">
         <v>6</v>
@@ -1386,19 +1386,19 @@
       <c r="F24" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="N24" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="O24" s="10"/>
+      <c r="N24" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="O24" s="7"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H25" t="s">
         <v>66</v>
       </c>
-      <c r="N25" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="O25" s="10"/>
+      <c r="N25" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="O25" s="7"/>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H26" s="1" t="s">
@@ -1407,10 +1407,10 @@
       <c r="I26" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N26" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="O26" s="10"/>
+      <c r="N26" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="O26" s="7"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H27" s="1" t="s">
@@ -1419,10 +1419,10 @@
       <c r="I27" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="N27" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="O27" s="10"/>
+      <c r="N27" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="O27" s="7"/>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H28" s="1" t="s">
@@ -1432,7 +1432,7 @@
         <v>6</v>
       </c>
       <c r="N28" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
@@ -1443,7 +1443,7 @@
         <v>6</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
@@ -1480,17 +1480,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="K20:L20"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="E9:F9"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="K20:L20"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>

</xml_diff>